<commit_message>
Create function displaying Project creation form ✔️
</commit_message>
<xml_diff>
--- a/Documentation/User_story.xlsx
+++ b/Documentation/User_story.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub victor-dva\you-form-doc\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD50856-A5A0-4DE0-BEC3-8A6C7797AAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D643C8-C9E5-4DD1-BD69-3315624C273F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1290" windowWidth="29040" windowHeight="15720" xr2:uid="{0D02B6C3-35DB-4657-970B-B42564126393}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="61">
   <si>
     <t>Story points</t>
   </si>
@@ -297,182 +297,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="22">
     <dxf>
       <fill>
         <patternFill>
@@ -526,6 +351,104 @@
       <fill>
         <patternFill>
           <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -849,7 +772,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,6 +1018,9 @@
       <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="F16" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
@@ -1110,7 +1036,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1600,41 +1526,41 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="cellIs" dxfId="24" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="6" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="between">
       <formula>1</formula>
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="11" operator="between">
       <formula>6</formula>
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="21" priority="8" operator="containsText" text="Tache">
+    <cfRule type="containsText" dxfId="18" priority="8" operator="containsText" text="Tache">
       <formula>NOT(ISERROR(SEARCH("Tache",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="9" operator="containsText" text="Technical story">
+    <cfRule type="containsText" dxfId="17" priority="9" operator="containsText" text="Technical story">
       <formula>NOT(ISERROR(SEARCH("Technical story",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="10" operator="containsText" text="User story">
+    <cfRule type="containsText" dxfId="16" priority="10" operator="containsText" text="User story">
       <formula>NOT(ISERROR(SEARCH("User story",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048576">
-    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="Todo">
-      <formula>NOT(ISERROR(SEARCH("Todo",F2)))</formula>
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="Validé">
+      <formula>NOT(ISERROR(SEARCH("Validé",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="Validé">
-      <formula>NOT(ISERROR(SEARCH("Validé",F2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",F2)))</formula>
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Todo">
+      <formula>NOT(ISERROR(SEARCH("Todo",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>